<commit_message>
新增 label and print
</commit_message>
<xml_diff>
--- a/Output/productivity_TL_April.xlsx
+++ b/Output/productivity_TL_April.xlsx
@@ -1021,13 +1021,13 @@
         <v>0</v>
       </c>
       <c r="S6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T6">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="U6">
-        <v>0.0392156862745098</v>
+        <v>0.02040816326530612</v>
       </c>
     </row>
     <row r="7" spans="1:21">
@@ -1080,13 +1080,13 @@
         <v>0</v>
       </c>
       <c r="S7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T7">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="U7">
-        <v>0.0425531914893617</v>
+        <v>0.02222222222222222</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -1552,13 +1552,13 @@
         <v>0</v>
       </c>
       <c r="S15">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="T15">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="U15">
-        <v>0.09803921568627451</v>
+        <v>0.08163265306122448</v>
       </c>
     </row>
     <row r="16" spans="1:21">
@@ -2440,10 +2440,10 @@
         <v>5</v>
       </c>
       <c r="T30">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="U30">
-        <v>0.119047619047619</v>
+        <v>0.1219512195121951</v>
       </c>
     </row>
     <row r="31" spans="1:21">
@@ -2499,10 +2499,10 @@
         <v>5</v>
       </c>
       <c r="T31">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="U31">
-        <v>0.119047619047619</v>
+        <v>0.1219512195121951</v>
       </c>
     </row>
     <row r="32" spans="1:21">
@@ -7632,10 +7632,10 @@
         <v>2</v>
       </c>
       <c r="T118">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="U118">
-        <v>0.04651162790697674</v>
+        <v>0.04878048780487805</v>
       </c>
     </row>
     <row r="119" spans="1:21">
@@ -7691,10 +7691,10 @@
         <v>2</v>
       </c>
       <c r="T119">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="U119">
-        <v>0.04651162790697674</v>
+        <v>0.04878048780487805</v>
       </c>
     </row>
     <row r="120" spans="1:21">
@@ -7809,10 +7809,10 @@
         <v>2</v>
       </c>
       <c r="T121">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="U121">
-        <v>0.04347826086956522</v>
+        <v>0.04545454545454546</v>
       </c>
     </row>
     <row r="122" spans="1:21">
@@ -7927,10 +7927,10 @@
         <v>5</v>
       </c>
       <c r="T123">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="U123">
-        <v>0.0847457627118644</v>
+        <v>0.08771929824561403</v>
       </c>
     </row>
     <row r="124" spans="1:21">
@@ -8163,10 +8163,10 @@
         <v>5</v>
       </c>
       <c r="T127">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="U127">
-        <v>0.0847457627118644</v>
+        <v>0.08771929824561403</v>
       </c>
     </row>
     <row r="128" spans="1:21">
@@ -8222,10 +8222,10 @@
         <v>5</v>
       </c>
       <c r="T128">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="U128">
-        <v>0.09615384615384616</v>
+        <v>0.09803921568627451</v>
       </c>
     </row>
     <row r="129" spans="1:21">
@@ -8576,10 +8576,10 @@
         <v>2</v>
       </c>
       <c r="T134">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="U134">
-        <v>0.0425531914893617</v>
+        <v>0.04444444444444445</v>
       </c>
     </row>
     <row r="135" spans="1:21">
@@ -9284,10 +9284,10 @@
         <v>11</v>
       </c>
       <c r="T146">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U146">
-        <v>0.180327868852459</v>
+        <v>0.1833333333333333</v>
       </c>
     </row>
     <row r="147" spans="1:21">
@@ -9343,10 +9343,10 @@
         <v>12</v>
       </c>
       <c r="T147">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="U147">
-        <v>0.1714285714285714</v>
+        <v>0.1764705882352941</v>
       </c>
     </row>
     <row r="148" spans="1:21">
@@ -9874,10 +9874,10 @@
         <v>4</v>
       </c>
       <c r="T156">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="U156">
-        <v>0.05882352941176471</v>
+        <v>0.06060606060606061</v>
       </c>
     </row>
     <row r="157" spans="1:21">
@@ -10110,10 +10110,10 @@
         <v>3</v>
       </c>
       <c r="T160">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="U160">
-        <v>0.04477611940298507</v>
+        <v>0.04615384615384616</v>
       </c>
     </row>
     <row r="161" spans="1:21">
@@ -10877,7 +10877,7 @@
         <v>0</v>
       </c>
       <c r="T173">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="U173">
         <v>0</v>
@@ -10936,10 +10936,10 @@
         <v>2</v>
       </c>
       <c r="T174">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="U174">
-        <v>0.02857142857142857</v>
+        <v>0.02941176470588235</v>
       </c>
     </row>
     <row r="175" spans="1:21">
@@ -11290,10 +11290,10 @@
         <v>1</v>
       </c>
       <c r="T180">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="U180">
-        <v>0.02325581395348837</v>
+        <v>0.02439024390243903</v>
       </c>
     </row>
     <row r="181" spans="1:21">
@@ -11467,10 +11467,10 @@
         <v>4</v>
       </c>
       <c r="T183">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="U183">
-        <v>0.06060606060606061</v>
+        <v>0.0625</v>
       </c>
     </row>
     <row r="184" spans="1:21">
@@ -11644,10 +11644,10 @@
         <v>4</v>
       </c>
       <c r="T186">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="U186">
-        <v>0.07407407407407407</v>
+        <v>0.07547169811320754</v>
       </c>
     </row>
     <row r="187" spans="1:21">
@@ -12408,13 +12408,13 @@
         <v>0</v>
       </c>
       <c r="S199">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T199">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="U199">
-        <v>0.02941176470588235</v>
+        <v>0</v>
       </c>
     </row>
     <row r="200" spans="1:21">
@@ -12526,13 +12526,13 @@
         <v>0</v>
       </c>
       <c r="S201">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T201">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="U201">
-        <v>0.03225806451612903</v>
+        <v>0</v>
       </c>
     </row>
     <row r="202" spans="1:21">
@@ -12703,13 +12703,13 @@
         <v>0</v>
       </c>
       <c r="S204">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="T204">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="U204">
-        <v>0.09090909090909091</v>
+        <v>0.04761904761904762</v>
       </c>
     </row>
     <row r="205" spans="1:21">
@@ -12762,13 +12762,13 @@
         <v>0</v>
       </c>
       <c r="S205">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T205">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="U205">
-        <v>0.1</v>
+        <v>0.07692307692307693</v>
       </c>
     </row>
     <row r="206" spans="1:21">
@@ -14830,10 +14830,10 @@
         <v>3</v>
       </c>
       <c r="T240">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="U240">
-        <v>0.08823529411764706</v>
+        <v>0.09375</v>
       </c>
     </row>
     <row r="241" spans="1:21">
@@ -15066,10 +15066,10 @@
         <v>7</v>
       </c>
       <c r="T244">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="U244">
-        <v>0.1458333333333333</v>
+        <v>0.1521739130434783</v>
       </c>
     </row>
     <row r="245" spans="1:21">
@@ -16125,13 +16125,13 @@
         <v>0</v>
       </c>
       <c r="S262">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T262">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="U262">
-        <v>0.07142857142857142</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="263" spans="1:21">
@@ -17246,13 +17246,13 @@
         <v>0</v>
       </c>
       <c r="S281">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T281">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="U281">
-        <v>0.05660377358490566</v>
+        <v>0.0392156862745098</v>
       </c>
     </row>
     <row r="282" spans="1:21">
@@ -17541,13 +17541,13 @@
         <v>0</v>
       </c>
       <c r="S286">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T286">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="U286">
-        <v>0.07272727272727272</v>
+        <v>0.05555555555555555</v>
       </c>
     </row>
     <row r="287" spans="1:21">
@@ -18249,13 +18249,13 @@
         <v>0</v>
       </c>
       <c r="S298">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T298">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="U298">
-        <v>0.02083333333333333</v>
+        <v>0</v>
       </c>
     </row>
     <row r="299" spans="1:21">
@@ -18308,13 +18308,13 @@
         <v>0</v>
       </c>
       <c r="S299">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T299">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="U299">
-        <v>0.02325581395348837</v>
+        <v>0</v>
       </c>
     </row>
     <row r="300" spans="1:21">
@@ -18606,10 +18606,10 @@
         <v>2</v>
       </c>
       <c r="T304">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="U304">
-        <v>0.03278688524590164</v>
+        <v>0.03389830508474576</v>
       </c>
     </row>
     <row r="305" spans="1:21">
@@ -18665,10 +18665,10 @@
         <v>2</v>
       </c>
       <c r="T305">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="U305">
-        <v>0.03333333333333333</v>
+        <v>0.03448275862068965</v>
       </c>
     </row>
     <row r="306" spans="1:21">
@@ -19550,10 +19550,10 @@
         <v>5</v>
       </c>
       <c r="T320">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="U320">
-        <v>0.125</v>
+        <v>0.1282051282051282</v>
       </c>
     </row>
     <row r="321" spans="1:21">
@@ -19609,10 +19609,10 @@
         <v>5</v>
       </c>
       <c r="T321">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="U321">
-        <v>0.1428571428571428</v>
+        <v>0.1470588235294118</v>
       </c>
     </row>
     <row r="322" spans="1:21">
@@ -19904,10 +19904,10 @@
         <v>5</v>
       </c>
       <c r="T326">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="U326">
-        <v>0.09259259259259259</v>
+        <v>0.09433962264150944</v>
       </c>
     </row>
     <row r="327" spans="1:21">
@@ -20081,10 +20081,10 @@
         <v>4</v>
       </c>
       <c r="T329">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="U329">
-        <v>0.07692307692307693</v>
+        <v>0.07843137254901961</v>
       </c>
     </row>
     <row r="330" spans="1:21">
@@ -24152,10 +24152,10 @@
         <v>2</v>
       </c>
       <c r="T398">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="U398">
-        <v>0.0625</v>
+        <v>0.06451612903225806</v>
       </c>
     </row>
     <row r="399" spans="1:21">
@@ -25332,10 +25332,10 @@
         <v>4</v>
       </c>
       <c r="T418">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="U418">
-        <v>0.06666666666666667</v>
+        <v>0.06896551724137931</v>
       </c>
     </row>
     <row r="419" spans="1:21">
@@ -26217,10 +26217,10 @@
         <v>1</v>
       </c>
       <c r="T433">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="U433">
-        <v>0.0303030303030303</v>
+        <v>0.03125</v>
       </c>
     </row>
     <row r="434" spans="1:21">
@@ -26335,10 +26335,10 @@
         <v>2</v>
       </c>
       <c r="T435">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="U435">
-        <v>0.03846153846153846</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="436" spans="1:21">
@@ -27043,10 +27043,10 @@
         <v>2</v>
       </c>
       <c r="T447">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="U447">
-        <v>0.05555555555555555</v>
+        <v>0.06060606060606061</v>
       </c>
     </row>
     <row r="448" spans="1:21">
@@ -27099,13 +27099,13 @@
         <v>0</v>
       </c>
       <c r="S448">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T448">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="U448">
-        <v>0.08888888888888889</v>
+        <v>0.07142857142857142</v>
       </c>
     </row>
     <row r="449" spans="1:21">
@@ -27276,13 +27276,13 @@
         <v>0</v>
       </c>
       <c r="S451">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="T451">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="U451">
-        <v>0.1228070175438596</v>
+        <v>0.1111111111111111</v>
       </c>
     </row>
     <row r="452" spans="1:21">
@@ -27394,13 +27394,13 @@
         <v>0</v>
       </c>
       <c r="S453">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="T453">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="U453">
-        <v>0.18</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="454" spans="1:21">
@@ -28102,13 +28102,13 @@
         <v>0</v>
       </c>
       <c r="S465">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T465">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="U465">
-        <v>0.03571428571428571</v>
+        <v>0</v>
       </c>
     </row>
     <row r="466" spans="1:21">
@@ -28161,13 +28161,13 @@
         <v>0</v>
       </c>
       <c r="S466">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T466">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="U466">
-        <v>0.04166666666666666</v>
+        <v>0</v>
       </c>
     </row>
     <row r="467" spans="1:21">
@@ -28459,10 +28459,10 @@
         <v>1</v>
       </c>
       <c r="T471">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="U471">
-        <v>0.02040816326530612</v>
+        <v>0.02173913043478261</v>
       </c>
     </row>
     <row r="472" spans="1:21">
@@ -28518,10 +28518,10 @@
         <v>1</v>
       </c>
       <c r="T472">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="U472">
-        <v>0.02040816326530612</v>
+        <v>0.02173913043478261</v>
       </c>
     </row>
     <row r="473" spans="1:21">
@@ -29344,10 +29344,10 @@
         <v>2</v>
       </c>
       <c r="T486">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="U486">
-        <v>0.05405405405405406</v>
+        <v>0.05882352941176471</v>
       </c>
     </row>
     <row r="487" spans="1:21">
@@ -29403,10 +29403,10 @@
         <v>2</v>
       </c>
       <c r="T487">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="U487">
-        <v>0.04878048780487805</v>
+        <v>0.05405405405405406</v>
       </c>
     </row>
     <row r="488" spans="1:21">
@@ -29757,10 +29757,10 @@
         <v>4</v>
       </c>
       <c r="T493">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="U493">
-        <v>0.07407407407407407</v>
+        <v>0.07692307692307693</v>
       </c>
     </row>
     <row r="494" spans="1:21">
@@ -29993,10 +29993,10 @@
         <v>4</v>
       </c>
       <c r="T497">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="U497">
-        <v>0.08</v>
+        <v>0.08163265306122448</v>
       </c>
     </row>
     <row r="498" spans="1:21">
@@ -31999,10 +31999,10 @@
         <v>1</v>
       </c>
       <c r="T531">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="U531">
-        <v>0.05555555555555555</v>
+        <v>0.05882352941176471</v>
       </c>
     </row>
     <row r="532" spans="1:21">
@@ -32763,13 +32763,13 @@
         <v>0</v>
       </c>
       <c r="S544">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T544">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="U544">
-        <v>0.03225806451612903</v>
+        <v>0</v>
       </c>
     </row>
     <row r="545" spans="1:21">
@@ -32943,10 +32943,10 @@
         <v>5</v>
       </c>
       <c r="T547">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="U547">
-        <v>0.125</v>
+        <v>0.1282051282051282</v>
       </c>
     </row>
     <row r="548" spans="1:21">
@@ -33651,10 +33651,10 @@
         <v>1</v>
       </c>
       <c r="T559">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="U559">
-        <v>0.02272727272727273</v>
+        <v>0.02380952380952381</v>
       </c>
     </row>
     <row r="560" spans="1:21">
@@ -33946,7 +33946,7 @@
         <v>0</v>
       </c>
       <c r="T564">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="U564">
         <v>0</v>
@@ -34831,7 +34831,7 @@
         <v>0</v>
       </c>
       <c r="T579">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="U579">
         <v>0</v>
@@ -35064,13 +35064,13 @@
         <v>0</v>
       </c>
       <c r="S583">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T583">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="U583">
-        <v>0.04166666666666666</v>
+        <v>0.02173913043478261</v>
       </c>
     </row>
     <row r="584" spans="1:21">
@@ -35952,7 +35952,7 @@
         <v>0</v>
       </c>
       <c r="T598">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="U598">
         <v>0</v>
@@ -36011,7 +36011,7 @@
         <v>0</v>
       </c>
       <c r="T599">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="U599">
         <v>0</v>
@@ -36424,10 +36424,10 @@
         <v>3</v>
       </c>
       <c r="T606">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="U606">
-        <v>0.05660377358490566</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="607" spans="1:21">
@@ -37309,10 +37309,10 @@
         <v>4</v>
       </c>
       <c r="T621">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="U621">
-        <v>0.09302325581395349</v>
+        <v>0.0975609756097561</v>
       </c>
     </row>
     <row r="622" spans="1:21">
@@ -37368,10 +37368,10 @@
         <v>4</v>
       </c>
       <c r="T622">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="U622">
-        <v>0.1</v>
+        <v>0.1052631578947368</v>
       </c>
     </row>
     <row r="623" spans="1:21">
@@ -37486,10 +37486,10 @@
         <v>2</v>
       </c>
       <c r="T624">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="U624">
-        <v>0.04545454545454546</v>
+        <v>0.04651162790697674</v>
       </c>
     </row>
     <row r="625" spans="1:21">
@@ -37663,10 +37663,10 @@
         <v>2</v>
       </c>
       <c r="T627">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="U627">
-        <v>0.04878048780487805</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="628" spans="1:21">
@@ -38453,10 +38453,10 @@
         <v>7</v>
       </c>
       <c r="G14">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="H14">
-        <v>0.06666666666666667</v>
+        <v>0.06930693069306931</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -38479,10 +38479,10 @@
         <v>5</v>
       </c>
       <c r="G15">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="H15">
-        <v>0.03164556962025317</v>
+        <v>0.03267973856209151</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -38502,13 +38502,13 @@
         <v>7.450000000000001</v>
       </c>
       <c r="F16">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G16">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="H16">
-        <v>0.0660377358490566</v>
+        <v>0.0392156862745098</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -38531,10 +38531,10 @@
         <v>16</v>
       </c>
       <c r="G17">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="H17">
-        <v>0.1322314049586777</v>
+        <v>0.1367521367521368</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -38554,13 +38554,13 @@
         <v>9.6</v>
       </c>
       <c r="F18">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G18">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H18">
-        <v>0.08870967741935484</v>
+        <v>0.08196721311475409</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -38580,13 +38580,13 @@
         <v>10.06666666666667</v>
       </c>
       <c r="F19">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G19">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="H19">
-        <v>0.06481481481481481</v>
+        <v>0.04761904761904762</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -38661,10 +38661,10 @@
         <v>9</v>
       </c>
       <c r="G22">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H22">
-        <v>0.08737864077669903</v>
+        <v>0.08823529411764706</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -38687,10 +38687,10 @@
         <v>4</v>
       </c>
       <c r="G23">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H23">
-        <v>0.06666666666666667</v>
+        <v>0.06896551724137931</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -38713,10 +38713,10 @@
         <v>3</v>
       </c>
       <c r="G24">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H24">
-        <v>0.03529411764705882</v>
+        <v>0.03658536585365853</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -38765,10 +38765,10 @@
         <v>3</v>
       </c>
       <c r="G26">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H26">
-        <v>0.05263157894736842</v>
+        <v>0.05357142857142857</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -38788,13 +38788,13 @@
         <v>8.916666666666666</v>
       </c>
       <c r="F27">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G27">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H27">
-        <v>0.06896551724137931</v>
+        <v>0.06194690265486726</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -39620,13 +39620,13 @@
         <v>9.25</v>
       </c>
       <c r="F59">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G59">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="H59">
-        <v>0.06862745098039216</v>
+        <v>0.05102040816326531</v>
       </c>
     </row>
     <row r="60" spans="1:8">
@@ -39649,10 +39649,10 @@
         <v>8</v>
       </c>
       <c r="G60">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H60">
-        <v>0.09523809523809523</v>
+        <v>0.0963855421686747</v>
       </c>
     </row>
     <row r="61" spans="1:8">
@@ -39701,10 +39701,10 @@
         <v>7</v>
       </c>
       <c r="G62">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="H62">
-        <v>0.06862745098039216</v>
+        <v>0.07142857142857142</v>
       </c>
     </row>
     <row r="63" spans="1:8">
@@ -39727,10 +39727,10 @@
         <v>16</v>
       </c>
       <c r="G63">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="H63">
-        <v>0.1159420289855072</v>
+        <v>0.1194029850746269</v>
       </c>
     </row>
     <row r="64" spans="1:8">
@@ -39753,10 +39753,10 @@
         <v>6</v>
       </c>
       <c r="G64">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="H64">
-        <v>0.04411764705882353</v>
+        <v>0.04545454545454546</v>
       </c>
     </row>
     <row r="65" spans="1:8">
@@ -39776,13 +39776,13 @@
         <v>10.23333333333333</v>
       </c>
       <c r="F65">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G65">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="H65">
-        <v>0.02777777777777778</v>
+        <v>0.01923076923076923</v>
       </c>
     </row>
     <row r="66" spans="1:8">
@@ -39805,10 +39805,10 @@
         <v>9</v>
       </c>
       <c r="G66">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H66">
-        <v>0.09782608695652174</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="67" spans="1:8">
@@ -39854,13 +39854,13 @@
         <v>10.2</v>
       </c>
       <c r="F68">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G68">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="H68">
-        <v>0.1368421052631579</v>
+        <v>0.1222222222222222</v>
       </c>
     </row>
     <row r="69" spans="1:8">
@@ -39880,13 +39880,13 @@
         <v>10.31666666666667</v>
       </c>
       <c r="F69">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G69">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="H69">
-        <v>0.02597402597402598</v>
+        <v>0.01408450704225352</v>
       </c>
     </row>
     <row r="70" spans="1:8">
@@ -39909,10 +39909,10 @@
         <v>6</v>
       </c>
       <c r="G70">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="H70">
-        <v>0.06593406593406594</v>
+        <v>0.06976744186046512</v>
       </c>
     </row>
     <row r="71" spans="1:8">
@@ -39935,10 +39935,10 @@
         <v>1</v>
       </c>
       <c r="G71">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="H71">
-        <v>0.009900990099009901</v>
+        <v>0.01030927835051546</v>
       </c>
     </row>
     <row r="72" spans="1:8">
@@ -39958,13 +39958,13 @@
         <v>10.4</v>
       </c>
       <c r="F72">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G72">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="H72">
-        <v>0.02105263157894737</v>
+        <v>0.01098901098901099</v>
       </c>
     </row>
     <row r="73" spans="1:8">
@@ -39987,10 +39987,10 @@
         <v>3</v>
       </c>
       <c r="G73">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="H73">
-        <v>0.03092783505154639</v>
+        <v>0.03296703296703297</v>
       </c>
     </row>
     <row r="74" spans="1:8">
@@ -40013,10 +40013,10 @@
         <v>6</v>
       </c>
       <c r="G74">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H74">
-        <v>0.07142857142857142</v>
+        <v>0.07407407407407407</v>
       </c>
     </row>
     <row r="75" spans="1:8">
@@ -42272,13 +42272,13 @@
         <v>3.133333333333333</v>
       </c>
       <c r="F161">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G161">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H161">
-        <v>0.0425531914893617</v>
+        <v>0.02222222222222222</v>
       </c>
     </row>
     <row r="162" spans="1:8">
@@ -42301,10 +42301,10 @@
         <v>7</v>
       </c>
       <c r="G162">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H162">
-        <v>0.08536585365853659</v>
+        <v>0.08641975308641975</v>
       </c>
     </row>
     <row r="163" spans="1:8">
@@ -42327,10 +42327,10 @@
         <v>9</v>
       </c>
       <c r="G163">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="H163">
-        <v>0.06338028169014084</v>
+        <v>0.06569343065693431</v>
       </c>
     </row>
     <row r="164" spans="1:8">
@@ -42353,10 +42353,10 @@
         <v>14</v>
       </c>
       <c r="G164">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="H164">
-        <v>0.109375</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="165" spans="1:8">
@@ -42376,13 +42376,13 @@
         <v>6.283333333333333</v>
       </c>
       <c r="F165">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G165">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="H165">
-        <v>0.06756756756756757</v>
+        <v>0.04225352112676056</v>
       </c>
     </row>
     <row r="166" spans="1:8">
@@ -42402,13 +42402,13 @@
         <v>10.15</v>
       </c>
       <c r="F166">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G166">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="H166">
-        <v>0.02884615384615385</v>
+        <v>0.0198019801980198</v>
       </c>
     </row>
     <row r="167" spans="1:8">
@@ -42431,10 +42431,10 @@
         <v>10</v>
       </c>
       <c r="G167">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H167">
-        <v>0.1123595505617977</v>
+        <v>0.1149425287356322</v>
       </c>
     </row>
     <row r="168" spans="1:8">
@@ -42480,13 +42480,13 @@
         <v>10.11666666666667</v>
       </c>
       <c r="F169">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G169">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="H169">
-        <v>0.09677419354838709</v>
+        <v>0.09195402298850575</v>
       </c>
     </row>
     <row r="170" spans="1:8">
@@ -42506,13 +42506,13 @@
         <v>10.18333333333333</v>
       </c>
       <c r="F170">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G170">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="H170">
-        <v>0.0273972602739726</v>
+        <v>0.01470588235294118</v>
       </c>
     </row>
     <row r="171" spans="1:8">
@@ -42535,10 +42535,10 @@
         <v>6</v>
       </c>
       <c r="G171">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="H171">
-        <v>0.06593406593406594</v>
+        <v>0.06976744186046512</v>
       </c>
     </row>
     <row r="172" spans="1:8">
@@ -42561,10 +42561,10 @@
         <v>2</v>
       </c>
       <c r="G172">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="H172">
-        <v>0.02298850574712644</v>
+        <v>0.02380952380952381</v>
       </c>
     </row>
     <row r="173" spans="1:8">
@@ -42587,10 +42587,10 @@
         <v>6</v>
       </c>
       <c r="G173">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H173">
-        <v>0.07142857142857142</v>
+        <v>0.07407407407407407</v>
       </c>
     </row>
     <row r="174" spans="1:8">
@@ -46389,7 +46389,7 @@
         <v>18</v>
       </c>
       <c r="D3">
-        <v>0.07288442131058068</v>
+        <v>0.07042902524650255</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -46431,7 +46431,7 @@
         <v>16</v>
       </c>
       <c r="D6">
-        <v>0.05645585539898487</v>
+        <v>0.0537758320064344</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -46557,7 +46557,7 @@
         <v>13</v>
       </c>
       <c r="D15">
-        <v>0.06476693813428322</v>
+        <v>0.06043418316242299</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -46923,43 +46923,43 @@
         <v>83</v>
       </c>
       <c r="I5">
-        <v>0.06666666666666667</v>
+        <v>0.06930693069306931</v>
       </c>
       <c r="K5">
-        <v>0.03164556962025317</v>
+        <v>0.03267973856209151</v>
       </c>
       <c r="L5">
-        <v>0.0660377358490566</v>
+        <v>0.0392156862745098</v>
       </c>
       <c r="N5">
-        <v>0.1322314049586777</v>
+        <v>0.1367521367521368</v>
       </c>
       <c r="O5">
-        <v>0.08870967741935484</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="P5">
-        <v>0.06481481481481481</v>
+        <v>0.04761904761904762</v>
       </c>
       <c r="T5">
         <v>0</v>
       </c>
       <c r="U5">
-        <v>0.08737864077669903</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="V5">
-        <v>0.06666666666666667</v>
+        <v>0.06896551724137931</v>
       </c>
       <c r="W5">
-        <v>0.03529411764705882</v>
+        <v>0.03658536585365853</v>
       </c>
       <c r="AA5">
         <v>0.01754385964912281</v>
       </c>
       <c r="AB5">
-        <v>0.05263157894736842</v>
+        <v>0.05357142857142857</v>
       </c>
       <c r="AC5">
-        <v>0.06896551724137931</v>
+        <v>0.06194690265486726</v>
       </c>
       <c r="AH5">
         <v>13</v>
@@ -47114,49 +47114,49 @@
         <v>83</v>
       </c>
       <c r="D9">
-        <v>0.06862745098039216</v>
+        <v>0.05102040816326531</v>
       </c>
       <c r="E9">
-        <v>0.09523809523809523</v>
+        <v>0.0963855421686747</v>
       </c>
       <c r="I9">
-        <v>0.06862745098039216</v>
+        <v>0.07142857142857142</v>
       </c>
       <c r="J9">
-        <v>0.1159420289855072</v>
+        <v>0.1194029850746269</v>
       </c>
       <c r="K9">
-        <v>0.04411764705882353</v>
+        <v>0.04545454545454546</v>
       </c>
       <c r="Q9">
-        <v>0.02777777777777778</v>
+        <v>0.01923076923076923</v>
       </c>
       <c r="R9">
-        <v>0.09782608695652174</v>
+        <v>0.1</v>
       </c>
       <c r="S9">
         <v>0.02307692307692308</v>
       </c>
       <c r="X9">
-        <v>0.1368421052631579</v>
+        <v>0.1222222222222222</v>
       </c>
       <c r="Y9">
-        <v>0.02597402597402598</v>
+        <v>0.01408450704225352</v>
       </c>
       <c r="Z9">
-        <v>0.06593406593406594</v>
+        <v>0.06976744186046512</v>
       </c>
       <c r="AD9">
-        <v>0.009900990099009901</v>
+        <v>0.01030927835051546</v>
       </c>
       <c r="AE9">
-        <v>0.02105263157894737</v>
+        <v>0.01098901098901099</v>
       </c>
       <c r="AF9">
-        <v>0.03092783505154639</v>
+        <v>0.03296703296703297</v>
       </c>
       <c r="AG9">
-        <v>0.07142857142857142</v>
+        <v>0.07407407407407407</v>
       </c>
       <c r="AH9">
         <v>15</v>
@@ -47543,43 +47543,43 @@
         <v>83</v>
       </c>
       <c r="D18">
-        <v>0.0425531914893617</v>
+        <v>0.02222222222222222</v>
       </c>
       <c r="E18">
-        <v>0.08536585365853659</v>
+        <v>0.08641975308641975</v>
       </c>
       <c r="I18">
-        <v>0.06338028169014084</v>
+        <v>0.06569343065693431</v>
       </c>
       <c r="J18">
-        <v>0.109375</v>
+        <v>0.112</v>
       </c>
       <c r="L18">
-        <v>0.06756756756756757</v>
+        <v>0.04225352112676056</v>
       </c>
       <c r="Q18">
-        <v>0.02884615384615385</v>
+        <v>0.0198019801980198</v>
       </c>
       <c r="R18">
-        <v>0.1123595505617977</v>
+        <v>0.1149425287356322</v>
       </c>
       <c r="S18">
         <v>0.048</v>
       </c>
       <c r="X18">
-        <v>0.09677419354838709</v>
+        <v>0.09195402298850575</v>
       </c>
       <c r="Y18">
-        <v>0.0273972602739726</v>
+        <v>0.01470588235294118</v>
       </c>
       <c r="Z18">
-        <v>0.06593406593406594</v>
+        <v>0.06976744186046512</v>
       </c>
       <c r="AF18">
-        <v>0.02298850574712644</v>
+        <v>0.02380952380952381</v>
       </c>
       <c r="AG18">
-        <v>0.07142857142857142</v>
+        <v>0.07407407407407407</v>
       </c>
       <c r="AH18">
         <v>13</v>

</xml_diff>